<commit_message>
plots added, sloppy final_plot_code.py for plotting and additional data analysis functions (probably should clean up), and minor modifications to other code to fit needs.
</commit_message>
<xml_diff>
--- a/reports/baseline_weather_models_results.xlsx
+++ b/reports/baseline_weather_models_results.xlsx
@@ -7300,16 +7300,16 @@
         <v>717</v>
       </c>
       <c r="C3">
-        <v>0.00291411003363462</v>
+        <v>0.002815893102647626</v>
       </c>
       <c r="D3">
-        <v>0.002355518498639464</v>
+        <v>0.002363450222930163</v>
       </c>
       <c r="E3">
-        <v>1787</v>
+        <v>2206</v>
       </c>
       <c r="F3">
-        <v>-2.413543365103763</v>
+        <v>-1.98727638272206</v>
       </c>
       <c r="G3" t="s">
         <v>719</v>
@@ -7318,7 +7318,7 @@
         <v>727</v>
       </c>
       <c r="I3">
-        <v>0.02248548976290904</v>
+        <v>0.01267744676585842</v>
       </c>
     </row>
     <row r="4" spans="1:705">
@@ -7442,16 +7442,16 @@
         <v>717</v>
       </c>
       <c r="C8">
-        <v>0.006905743167593736</v>
+        <v>0.005617109956273847</v>
       </c>
       <c r="D8">
-        <v>0.006349387841637189</v>
+        <v>0.005165938046090668</v>
       </c>
       <c r="E8">
-        <v>1787</v>
+        <v>2206</v>
       </c>
       <c r="F8">
-        <v>-0.9390129435767169</v>
+        <v>-0.8611730043194742</v>
       </c>
       <c r="G8" t="s">
         <v>724</v>
@@ -7460,7 +7460,7 @@
         <v>726</v>
       </c>
       <c r="I8">
-        <v>0.0004372118804737192</v>
+        <v>0.0004265388728027442</v>
       </c>
     </row>
     <row r="9" spans="1:705">
@@ -7538,31 +7538,31 @@
         <v>717</v>
       </c>
       <c r="C11">
-        <v>0.00392045576339195</v>
+        <v>0.003597226888345073</v>
       </c>
       <c r="D11">
-        <v>0.002803774659987601</v>
+        <v>0.002692639713481992</v>
       </c>
       <c r="E11">
-        <v>1787</v>
+        <v>2206</v>
       </c>
       <c r="F11">
-        <v>3.123999046168083</v>
+        <v>0.8557137033339899</v>
       </c>
       <c r="G11" t="s">
         <v>719</v>
       </c>
       <c r="I11">
-        <v>0.4632261470098115</v>
+        <v>0.7104956551870635</v>
       </c>
       <c r="J11">
-        <v>0.4278958612571066</v>
+        <v>0.2748856456563241</v>
       </c>
       <c r="K11" t="s">
         <v>730</v>
       </c>
       <c r="M11">
-        <v>0.1795949922259763</v>
+        <v>0.1888682689552658</v>
       </c>
     </row>
     <row r="12" spans="1:705">
@@ -7716,16 +7716,16 @@
         <v>912</v>
       </c>
       <c r="B2">
-        <v>-2.418818049127605</v>
+        <v>-9.597644919092192</v>
       </c>
       <c r="C2">
-        <v>12.64235753295049</v>
+        <v>5.560270364463445</v>
       </c>
       <c r="D2">
-        <v>-0.1913265024203994</v>
+        <v>-1.726111194238366</v>
       </c>
       <c r="E2">
-        <v>0.8482915704542207</v>
+        <v>0.08446761919523635</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -7733,16 +7733,16 @@
         <v>719</v>
       </c>
       <c r="B3">
-        <v>3.123999046168083</v>
+        <v>0.8557137033339899</v>
       </c>
       <c r="C3">
-        <v>4.257852069475423</v>
+        <v>2.305024620451809</v>
       </c>
       <c r="D3">
-        <v>0.7337030491416219</v>
+        <v>0.3712384222456855</v>
       </c>
       <c r="E3">
-        <v>0.4632261470098115</v>
+        <v>0.7104956551870635</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -7750,16 +7750,16 @@
         <v>730</v>
       </c>
       <c r="B4">
-        <v>0.4278958612571066</v>
+        <v>0.2748856456563241</v>
       </c>
       <c r="C4">
-        <v>0.3187234865097047</v>
+        <v>0.2091433090156062</v>
       </c>
       <c r="D4">
-        <v>1.342530059340568</v>
+        <v>1.314341094391942</v>
       </c>
       <c r="E4">
-        <v>0.1795949922259763</v>
+        <v>0.1888682689552658</v>
       </c>
     </row>
   </sheetData>
@@ -10883,16 +10883,16 @@
         <v>912</v>
       </c>
       <c r="B2">
-        <v>-16.76819468100025</v>
+        <v>-13.73881319106358</v>
       </c>
       <c r="C2">
-        <v>6.753498324310202</v>
+        <v>4.582168744596629</v>
       </c>
       <c r="D2">
-        <v>-2.482890181617531</v>
+        <v>-2.99832109135322</v>
       </c>
       <c r="E2">
-        <v>0.01312339238147633</v>
+        <v>0.002745071703381285</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -10900,16 +10900,16 @@
         <v>719</v>
       </c>
       <c r="B3">
-        <v>-2.413543365103763</v>
+        <v>-1.98727638272206</v>
       </c>
       <c r="C3">
-        <v>1.056694162531421</v>
+        <v>0.796584897355873</v>
       </c>
       <c r="D3">
-        <v>-2.284051006132057</v>
+        <v>-2.494745242244089</v>
       </c>
       <c r="E3">
-        <v>0.02248548976290904</v>
+        <v>0.01267744676585842</v>
       </c>
     </row>
   </sheetData>
@@ -11203,16 +11203,16 @@
         <v>912</v>
       </c>
       <c r="B2">
-        <v>25.93127612641543</v>
+        <v>23.05225985332796</v>
       </c>
       <c r="C2">
-        <v>8.697022084274426</v>
+        <v>8.254288016275737</v>
       </c>
       <c r="D2">
-        <v>2.981627029935135</v>
+        <v>2.792761750967946</v>
       </c>
       <c r="E2">
-        <v>0.002906023659063804</v>
+        <v>0.0052711407292965</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -11220,16 +11220,16 @@
         <v>724</v>
       </c>
       <c r="B3">
-        <v>-0.9390129435767169</v>
+        <v>-0.8611730043194742</v>
       </c>
       <c r="C3">
-        <v>0.2665277864651704</v>
+        <v>0.2440647003845162</v>
       </c>
       <c r="D3">
-        <v>-3.523133388943768</v>
+        <v>-3.52846193227748</v>
       </c>
       <c r="E3">
-        <v>0.0004372118804737192</v>
+        <v>0.0004265388728027442</v>
       </c>
     </row>
   </sheetData>

</xml_diff>